<commit_message>
all good but filters
</commit_message>
<xml_diff>
--- a/data/training/data_train.xlsx
+++ b/data/training/data_train.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marinamu\Documents\ASE_audio\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kennesawedu-my.sharepoint.com/personal/mnaser1_kennesaw_edu/Documents/Desktop/ASDSpeech-main - 2/data/training/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_B7F0A4C79D5226D54F78B000FD7C75AA9D769D15" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA413580-2494-41BC-AB41-97107181A524}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="31065" yWindow="2040" windowWidth="20010" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -603,8 +617,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -965,30 +979,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
+    <col min="6" max="6" width="4.44140625" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1026,7 +1040,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1064,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1102,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1140,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1178,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1216,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1254,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1292,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1330,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1368,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1406,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1444,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1482,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1520,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1596,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1628,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1666,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1704,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1742,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1774,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1812,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1850,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1888,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1926,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -1964,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2002,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2040,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -2078,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2116,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2154,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -2192,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -2230,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -2268,7 +2282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2306,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -2344,7 +2358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -2382,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>93</v>
       </c>
@@ -2420,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -2455,7 +2469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -2493,7 +2507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -2531,7 +2545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -2569,7 +2583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -2607,7 +2621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -2645,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -2683,7 +2697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2721,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>102</v>
       </c>
@@ -2759,7 +2773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -2797,7 +2811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -2835,7 +2849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -2873,7 +2887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -2911,7 +2925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2949,7 +2963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -2987,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3025,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -3063,7 +3077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -3101,7 +3115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -3139,7 +3153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -3177,7 +3191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -3215,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -3253,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>116</v>
       </c>
@@ -3291,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -3329,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3367,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>119</v>
       </c>
@@ -3405,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>120</v>
       </c>
@@ -3443,7 +3457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>121</v>
       </c>
@@ -3481,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -3519,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>123</v>
       </c>
@@ -3557,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>124</v>
       </c>
@@ -3595,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -3633,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>126</v>
       </c>
@@ -3671,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>127</v>
       </c>
@@ -3709,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>128</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>129</v>
       </c>
@@ -3785,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>130</v>
       </c>
@@ -3823,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>131</v>
       </c>
@@ -3861,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>132</v>
       </c>
@@ -3899,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>133</v>
       </c>
@@ -3937,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>134</v>
       </c>
@@ -3975,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>135</v>
       </c>
@@ -4013,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>136</v>
       </c>
@@ -4051,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>137</v>
       </c>
@@ -4089,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>138</v>
       </c>
@@ -4127,7 +4141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>139</v>
       </c>
@@ -4165,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>140</v>
       </c>
@@ -4203,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -4241,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>142</v>
       </c>
@@ -4279,7 +4293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -4317,7 +4331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>144</v>
       </c>
@@ -4355,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>145</v>
       </c>
@@ -4393,7 +4407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>146</v>
       </c>
@@ -4431,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>147</v>
       </c>
@@ -4469,7 +4483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>148</v>
       </c>
@@ -4507,7 +4521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>149</v>
       </c>
@@ -4545,7 +4559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>150</v>
       </c>
@@ -4583,7 +4597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -4621,7 +4635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>152</v>
       </c>
@@ -4659,7 +4673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>153</v>
       </c>
@@ -4697,7 +4711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>154</v>
       </c>
@@ -4732,7 +4746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>155</v>
       </c>
@@ -4770,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>156</v>
       </c>
@@ -4808,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>157</v>
       </c>
@@ -4846,7 +4860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>158</v>
       </c>
@@ -4884,7 +4898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>159</v>
       </c>
@@ -4922,7 +4936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>160</v>
       </c>
@@ -4960,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>161</v>
       </c>
@@ -4998,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>162</v>
       </c>
@@ -5036,7 +5050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>163</v>
       </c>
@@ -5074,7 +5088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>164</v>
       </c>
@@ -5112,7 +5126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>165</v>
       </c>
@@ -5150,7 +5164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>166</v>
       </c>
@@ -5188,7 +5202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>167</v>
       </c>
@@ -5226,7 +5240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>168</v>
       </c>
@@ -5264,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>169</v>
       </c>
@@ -5302,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>170</v>
       </c>
@@ -5340,7 +5354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>171</v>
       </c>
@@ -5378,7 +5392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>172</v>
       </c>
@@ -5416,7 +5430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>173</v>
       </c>
@@ -5454,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>174</v>
       </c>
@@ -5492,7 +5506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>175</v>
       </c>
@@ -5530,7 +5544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>176</v>
       </c>
@@ -5568,7 +5582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>177</v>
       </c>
@@ -5606,7 +5620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>178</v>
       </c>
@@ -5644,7 +5658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>179</v>
       </c>
@@ -5682,7 +5696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>180</v>
       </c>
@@ -5720,7 +5734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>181</v>
       </c>
@@ -5758,7 +5772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>182</v>
       </c>
@@ -5796,7 +5810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>183</v>
       </c>
@@ -5834,7 +5848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>184</v>
       </c>
@@ -5872,7 +5886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>185</v>
       </c>
@@ -5910,7 +5924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>186</v>
       </c>
@@ -5948,7 +5962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>187</v>
       </c>
@@ -5986,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>188</v>
       </c>
@@ -6024,7 +6038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>189</v>
       </c>
@@ -6062,7 +6076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>190</v>
       </c>
@@ -6100,7 +6114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>191</v>
       </c>
@@ -6138,7 +6152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>192</v>
       </c>

</xml_diff>